<commit_message>
Remove .pyc files from version control and add to .gitignore
</commit_message>
<xml_diff>
--- a/static/user_workout_DB/Users.xlsx
+++ b/static/user_workout_DB/Users.xlsx
@@ -9,6 +9,7 @@
     <sheet name="workout_data_ish" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="workout_data_johndoe20" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="workout_data_tvisha" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="workout_data_mahad123" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -1278,6 +1279,367 @@
       <c r="D3" t="n">
         <v>74.2</v>
       </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="5" t="n">
+        <v>45620</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>74.2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="5" t="n">
+        <v>45621</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>73.90000000000001</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="5" t="n">
+        <v>45622</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Legs</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>74.5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="5" t="n">
+        <v>45623</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>74.5</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="5" t="n">
+        <v>45624</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>74.5</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="5" t="n">
+        <v>45625</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Arms</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="5" t="n">
+        <v>45626</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Core</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>75.8</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="5" t="n">
+        <v>45627</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Chest</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="5" t="n">
+        <v>45628</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Chest</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>76.2</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="5" t="n">
+        <v>45629</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>76.2</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="5" t="n">
+        <v>45630</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Arms</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>76.8</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="5" t="n">
+        <v>45631</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>76.59999999999999</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="5" t="n">
+        <v>45632</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Chest</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>77.09999999999999</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="5" t="n">
+        <v>45633</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>77.09999999999999</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="5" t="n">
+        <v>45634</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Legs</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>77.09999999999999</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="5" t="n">
+        <v>45635</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>77.5</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="5" t="n">
+        <v>45636</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>77.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>Workout(Y/N)</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>Exercise_type</t>
+        </is>
+      </c>
+      <c r="D1" s="4" t="inlineStr">
+        <is>
+          <t>weight_record</t>
+        </is>
+      </c>
+      <c r="E1" s="4" t="inlineStr">
+        <is>
+          <t>height</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="5" t="n">
+        <v>45618</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Chest</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>74</v>
+      </c>
+      <c r="E2" t="n">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="n">
+        <v>45619</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Arms</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>74.2</v>
+      </c>
       <c r="E3" t="inlineStr"/>
     </row>
     <row r="4">

</xml_diff>